<commit_message>
Some Changes in Slice-CC
</commit_message>
<xml_diff>
--- a/media/MAGMA/Billing/FEB 22/Performance.xlsx
+++ b/media/MAGMA/Billing/FEB 22/Performance.xlsx
@@ -493,16 +493,16 @@
         <v>191</v>
       </c>
       <c r="E2" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>60058</v>
+        <v>53222</v>
       </c>
       <c r="H2" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3">
@@ -523,16 +523,16 @@
         <v>123</v>
       </c>
       <c r="E3" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="n">
-        <v>1043994.34</v>
+        <v>1059235.75</v>
       </c>
       <c r="H3" t="n">
-        <v>9.42</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="4">

</xml_diff>